<commit_message>
atualizacao do modulo gerar atas
</commit_message>
<xml_diff>
--- a/database/report_deserto_fracassado.xlsx
+++ b/database/report_deserto_fracassado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,119 +561,7 @@
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>descricao_detalhada_tr</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>791010</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>CENTRO DE INTENDENCIA DA MARINHA NITEROI</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>SRP - Registro de Preço</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Processo Licitatório para Aquisição de Materiais Elétricos</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>4</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>91.59999999999999</v>
-      </c>
-      <c r="J2" t="n">
-        <v>137</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Unidade</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Fracassado e Homologado</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="n">
-        <v>463692</v>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>ÓLEO VEGETAL COMESTÍVEL</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>ÓLEO VEGETAL COMESTÍVEL, TIPO: PURO, ESPÉCIE VEGETAL: SOJA, TIPO QUALIDADE: TIPO 1 (Frasco de 900ml)</t>
+          <t>descricao_detalhada</t>
         </is>
       </c>
     </row>

</xml_diff>